<commit_message>
Fixed a couple issues, cleaned up unit test structure a bit
</commit_message>
<xml_diff>
--- a/vfBattleTechMod-ProcGenStores-Test/res/xlrp-store-content.xlsx
+++ b/vfBattleTechMod-ProcGenStores-Test/res/xlrp-store-content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Weistra\gitrepos\vfBattleTechMod-Core\vfBattleTechMod-ProcGenStores-Test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5B3228C-7D64-4522-B7FE-5C7B5F563A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F8EBE0-0965-44E4-94DF-7FB8803BEA69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4275" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="544">
   <si>
     <t>ActuatorTemplate</t>
   </si>
@@ -613,231 +613,6 @@
   </si>
   <si>
     <t>emod_engine_030</t>
-  </si>
-  <si>
-    <t>emod_engine_035</t>
-  </si>
-  <si>
-    <t>emod_engine_040</t>
-  </si>
-  <si>
-    <t>emod_engine_045</t>
-  </si>
-  <si>
-    <t>emod_engine_050</t>
-  </si>
-  <si>
-    <t>emod_engine_055</t>
-  </si>
-  <si>
-    <t>emod_engine_060</t>
-  </si>
-  <si>
-    <t>emod_engine_065</t>
-  </si>
-  <si>
-    <t>emod_engine_070</t>
-  </si>
-  <si>
-    <t>emod_engine_075</t>
-  </si>
-  <si>
-    <t>emod_engine_080</t>
-  </si>
-  <si>
-    <t>emod_engine_085</t>
-  </si>
-  <si>
-    <t>emod_engine_090</t>
-  </si>
-  <si>
-    <t>emod_engine_095</t>
-  </si>
-  <si>
-    <t>emod_engine_100</t>
-  </si>
-  <si>
-    <t>emod_engine_105</t>
-  </si>
-  <si>
-    <t>emod_engine_110</t>
-  </si>
-  <si>
-    <t>emod_engine_115</t>
-  </si>
-  <si>
-    <t>emod_engine_120</t>
-  </si>
-  <si>
-    <t>emod_engine_125</t>
-  </si>
-  <si>
-    <t>emod_engine_130</t>
-  </si>
-  <si>
-    <t>emod_engine_135</t>
-  </si>
-  <si>
-    <t>emod_engine_140</t>
-  </si>
-  <si>
-    <t>emod_engine_145</t>
-  </si>
-  <si>
-    <t>emod_engine_150</t>
-  </si>
-  <si>
-    <t>emod_engine_155</t>
-  </si>
-  <si>
-    <t>emod_engine_160</t>
-  </si>
-  <si>
-    <t>emod_engine_165</t>
-  </si>
-  <si>
-    <t>emod_engine_170</t>
-  </si>
-  <si>
-    <t>emod_engine_175</t>
-  </si>
-  <si>
-    <t>emod_engine_180</t>
-  </si>
-  <si>
-    <t>emod_engine_185</t>
-  </si>
-  <si>
-    <t>emod_engine_190</t>
-  </si>
-  <si>
-    <t>emod_engine_195</t>
-  </si>
-  <si>
-    <t>emod_engine_200</t>
-  </si>
-  <si>
-    <t>emod_engine_205</t>
-  </si>
-  <si>
-    <t>emod_engine_210</t>
-  </si>
-  <si>
-    <t>emod_engine_215</t>
-  </si>
-  <si>
-    <t>emod_engine_220</t>
-  </si>
-  <si>
-    <t>emod_engine_225</t>
-  </si>
-  <si>
-    <t>emod_engine_230</t>
-  </si>
-  <si>
-    <t>emod_engine_235</t>
-  </si>
-  <si>
-    <t>emod_engine_240</t>
-  </si>
-  <si>
-    <t>emod_engine_245</t>
-  </si>
-  <si>
-    <t>emod_engine_250</t>
-  </si>
-  <si>
-    <t>emod_engine_255</t>
-  </si>
-  <si>
-    <t>emod_engine_260</t>
-  </si>
-  <si>
-    <t>emod_engine_265</t>
-  </si>
-  <si>
-    <t>emod_engine_270</t>
-  </si>
-  <si>
-    <t>emod_engine_275</t>
-  </si>
-  <si>
-    <t>emod_engine_280</t>
-  </si>
-  <si>
-    <t>emod_engine_285</t>
-  </si>
-  <si>
-    <t>emod_engine_290</t>
-  </si>
-  <si>
-    <t>emod_engine_295</t>
-  </si>
-  <si>
-    <t>emod_engine_300</t>
-  </si>
-  <si>
-    <t>emod_engine_305</t>
-  </si>
-  <si>
-    <t>emod_engine_310</t>
-  </si>
-  <si>
-    <t>emod_engine_315</t>
-  </si>
-  <si>
-    <t>emod_engine_320</t>
-  </si>
-  <si>
-    <t>emod_engine_325</t>
-  </si>
-  <si>
-    <t>emod_engine_330</t>
-  </si>
-  <si>
-    <t>emod_engine_335</t>
-  </si>
-  <si>
-    <t>emod_engine_340</t>
-  </si>
-  <si>
-    <t>emod_engine_345</t>
-  </si>
-  <si>
-    <t>emod_engine_350</t>
-  </si>
-  <si>
-    <t>emod_engine_355</t>
-  </si>
-  <si>
-    <t>emod_engine_360</t>
-  </si>
-  <si>
-    <t>emod_engine_365</t>
-  </si>
-  <si>
-    <t>emod_engine_370</t>
-  </si>
-  <si>
-    <t>emod_engine_375</t>
-  </si>
-  <si>
-    <t>emod_engine_380</t>
-  </si>
-  <si>
-    <t>emod_engine_385</t>
-  </si>
-  <si>
-    <t>emod_engine_390</t>
-  </si>
-  <si>
-    <t>emod_engine_395</t>
-  </si>
-  <si>
-    <t>emod_engine_400</t>
-  </si>
-  <si>
-    <t>emod_engine_9000</t>
   </si>
   <si>
     <t>emod_engine_cooling</t>
@@ -2364,248 +2139,248 @@
     <row r="1" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:6" ht="15.75" thickBot="1">
       <c r="B2" s="6" t="s">
-        <v>559</v>
+        <v>484</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>583</v>
+        <v>508</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>597</v>
+        <v>522</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>583</v>
+        <v>508</v>
       </c>
     </row>
     <row r="3" spans="2:6">
       <c r="B3" s="5" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>584</v>
+        <v>509</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>594</v>
+        <v>519</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>599</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="2:6">
       <c r="B4" s="3" t="s">
-        <v>552</v>
+        <v>477</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>585</v>
+        <v>510</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>595</v>
+        <v>520</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>600</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="2:6">
       <c r="B5" s="3" t="s">
-        <v>555</v>
+        <v>480</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>586</v>
+        <v>511</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>596</v>
+        <v>521</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>601</v>
+        <v>526</v>
       </c>
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="3" t="s">
-        <v>551</v>
+        <v>476</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>587</v>
+        <v>512</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>598</v>
+        <v>523</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>604</v>
+        <v>529</v>
       </c>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="3" t="s">
-        <v>553</v>
+        <v>478</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>588</v>
+        <v>513</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>605</v>
+        <v>530</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>606</v>
+        <v>531</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="3" t="s">
-        <v>556</v>
+        <v>481</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>589</v>
+        <v>514</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="3" t="s">
-        <v>550</v>
+        <v>475</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>590</v>
+        <v>515</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="3" t="s">
-        <v>557</v>
+        <v>482</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>591</v>
+        <v>516</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="3" t="s">
-        <v>558</v>
+        <v>483</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>592</v>
+        <v>517</v>
       </c>
     </row>
     <row r="12" spans="2:6" ht="15.75" thickBot="1">
       <c r="B12" s="4" t="s">
-        <v>554</v>
+        <v>479</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>593</v>
+        <v>518</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15.75" thickBot="1"/>
     <row r="14" spans="2:6" ht="15.75" thickBot="1">
       <c r="B14" s="9" t="s">
-        <v>560</v>
+        <v>485</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>603</v>
+        <v>528</v>
       </c>
     </row>
     <row r="15" spans="2:6" ht="30">
       <c r="B15" s="10" t="s">
-        <v>561</v>
+        <v>486</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>602</v>
+        <v>527</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="B16" s="11" t="s">
-        <v>562</v>
+        <v>487</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="12" t="s">
-        <v>563</v>
+        <v>488</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="12" t="s">
-        <v>564</v>
+        <v>489</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" s="12" t="s">
-        <v>565</v>
+        <v>490</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="11" t="s">
-        <v>566</v>
+        <v>491</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="30">
       <c r="B21" s="12" t="s">
-        <v>567</v>
+        <v>492</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="12" t="s">
-        <v>568</v>
+        <v>493</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" s="12" t="s">
-        <v>569</v>
+        <v>494</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="30">
       <c r="B24" s="12" t="s">
-        <v>570</v>
+        <v>495</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="30">
       <c r="B25" s="12" t="s">
-        <v>571</v>
+        <v>496</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" s="12" t="s">
-        <v>572</v>
+        <v>497</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" s="12" t="s">
-        <v>573</v>
+        <v>498</v>
       </c>
     </row>
     <row r="28" spans="2:2">
       <c r="B28" s="12" t="s">
-        <v>574</v>
+        <v>499</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" s="12" t="s">
-        <v>575</v>
+        <v>500</v>
       </c>
     </row>
     <row r="30" spans="2:2">
       <c r="B30" s="12" t="s">
-        <v>576</v>
+        <v>501</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" s="7" t="s">
-        <v>577</v>
+        <v>502</v>
       </c>
     </row>
     <row r="32" spans="2:2">
       <c r="B32" s="7" t="s">
-        <v>578</v>
+        <v>503</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" s="7" t="s">
-        <v>579</v>
+        <v>504</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" s="7" t="s">
-        <v>580</v>
+        <v>505</v>
       </c>
     </row>
     <row r="35" spans="2:2">
       <c r="B35" s="7" t="s">
-        <v>581</v>
+        <v>506</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" thickBot="1">
       <c r="B36" s="8" t="s">
-        <v>582</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -3607,11 +3382,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3627,28 +3402,28 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
-        <v>545</v>
+        <v>470</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>608</v>
+        <v>533</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>609</v>
+        <v>534</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>547</v>
+        <v>472</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>610</v>
+        <v>535</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>546</v>
+        <v>471</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>549</v>
+        <v>474</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>583</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -3656,22 +3431,22 @@
         <v>191</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>553</v>
+        <v>478</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -3679,22 +3454,22 @@
         <v>192</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>553</v>
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -3702,22 +3477,22 @@
         <v>193</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>553</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -3725,22 +3500,22 @@
         <v>194</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>553</v>
+        <v>478</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -3748,22 +3523,22 @@
         <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>553</v>
+        <v>478</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -3771,22 +3546,22 @@
         <v>196</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>553</v>
+        <v>473</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -3794,22 +3569,22 @@
         <v>197</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>553</v>
+        <v>476</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -3817,22 +3592,22 @@
         <v>198</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>553</v>
+        <v>476</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -3840,22 +3615,22 @@
         <v>199</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>553</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -3863,22 +3638,22 @@
         <v>200</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>553</v>
+        <v>476</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -3886,22 +3661,22 @@
         <v>201</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>553</v>
+        <v>476</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -3909,22 +3684,22 @@
         <v>202</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>553</v>
+        <v>476</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -3932,22 +3707,22 @@
         <v>203</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>553</v>
+        <v>476</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -3955,22 +3730,22 @@
         <v>204</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>553</v>
+        <v>473</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -3978,2072 +3753,347 @@
         <v>205</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>548</v>
+        <v>532</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
+      </c>
+      <c r="F16">
+        <v>3072</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>206</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>207</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>208</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>548</v>
+        <v>537</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>548</v>
+        <v>538</v>
+      </c>
+      <c r="D19">
+        <v>2865</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>548</v>
+        <v>539</v>
+      </c>
+      <c r="F19">
+        <v>3045</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>209</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>548</v>
+        <v>541</v>
+      </c>
+      <c r="D20">
+        <v>2865</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>548</v>
+        <v>542</v>
+      </c>
+      <c r="F20">
+        <v>3045</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>210</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>211</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>212</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>548</v>
+        <v>541</v>
+      </c>
+      <c r="D23">
+        <v>2865</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>548</v>
+        <v>542</v>
+      </c>
+      <c r="F23">
+        <v>3045</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>213</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>214</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>215</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>216</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>217</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>218</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>219</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" t="s">
-        <v>220</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>221</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>222</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>223</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" t="s">
-        <v>224</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>225</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
-      <c r="A37" t="s">
-        <v>226</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>227</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>228</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>229</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>230</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>231</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>232</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>233</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G44" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" t="s">
-        <v>234</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46" t="s">
-        <v>235</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G46" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" t="s">
-        <v>236</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G47" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48" t="s">
-        <v>237</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" t="s">
-        <v>238</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" t="s">
-        <v>239</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51" t="s">
-        <v>240</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52" t="s">
-        <v>241</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" t="s">
-        <v>242</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54" t="s">
-        <v>243</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
-        <v>244</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F55" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56" t="s">
-        <v>245</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7">
-      <c r="A57" t="s">
-        <v>246</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7">
-      <c r="A58" t="s">
-        <v>247</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7">
-      <c r="A59" t="s">
-        <v>248</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" t="s">
-        <v>249</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7">
-      <c r="A61" t="s">
-        <v>250</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" t="s">
-        <v>251</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7">
-      <c r="A63" t="s">
-        <v>252</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7">
-      <c r="A64" t="s">
-        <v>253</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
-      <c r="A65" t="s">
-        <v>254</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" t="s">
-        <v>255</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7">
-      <c r="A67" t="s">
-        <v>256</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7">
-      <c r="A68" t="s">
-        <v>257</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D68" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E68" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7">
-      <c r="A69" t="s">
-        <v>258</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C69" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7">
-      <c r="A70" t="s">
-        <v>259</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7">
-      <c r="A71" t="s">
-        <v>260</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C71" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F71" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7">
-      <c r="A72" t="s">
-        <v>261</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7">
-      <c r="A73" t="s">
-        <v>262</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
-      <c r="A74" t="s">
-        <v>263</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" t="s">
-        <v>264</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" t="s">
-        <v>265</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E76" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7">
-      <c r="A77" t="s">
-        <v>266</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E77" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7">
-      <c r="A78" t="s">
-        <v>267</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D78" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E78" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G78" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7">
-      <c r="A79" t="s">
-        <v>268</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E79" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F79" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G79" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7">
-      <c r="A80" t="s">
-        <v>269</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F80" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8">
-      <c r="A81" t="s">
-        <v>270</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F81" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8">
-      <c r="A82" t="s">
-        <v>271</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" t="s">
-        <v>272</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" t="s">
-        <v>273</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E84" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G84" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" t="s">
-        <v>274</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F85" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" t="s">
-        <v>275</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E86" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F86" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G86" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" t="s">
-        <v>276</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F87" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G87" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" t="s">
-        <v>277</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F88" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G88" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" t="s">
-        <v>278</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G89" s="2" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8">
-      <c r="A90" t="s">
-        <v>279</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C90" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E90" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F90" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" t="s">
-        <v>280</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="C91" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="D91" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E91" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F91">
-        <v>3072</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8">
-      <c r="A92" t="s">
-        <v>281</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="A93" t="s">
-        <v>282</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C93" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D93" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F93" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G93" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" t="s">
-        <v>283</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="C94" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="D94">
-        <v>2865</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="F94">
-        <v>3045</v>
-      </c>
-      <c r="G94" s="2" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="A95" t="s">
-        <v>284</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="D95">
-        <v>2865</v>
-      </c>
-      <c r="E95" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="F95">
-        <v>3045</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="A96" t="s">
-        <v>285</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D96" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F96" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G96" s="2" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7">
-      <c r="A97" t="s">
-        <v>286</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D97" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E97" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F97" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7">
-      <c r="A98" t="s">
-        <v>287</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="C98" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="D98">
-        <v>2865</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="F98">
-        <v>3045</v>
-      </c>
-      <c r="G98" s="2" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
-      <c r="A99" t="s">
-        <v>288</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D99" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E99" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F99" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G99" s="2" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" t="s">
-        <v>289</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G100" s="2" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
-      <c r="A101" t="s">
-        <v>290</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C101" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D101" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G101" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7">
-      <c r="A102" t="s">
-        <v>291</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D102" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F102" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G102" s="2" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" t="s">
-        <v>292</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C103" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D103" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F103" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G103" s="2" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" t="s">
-        <v>293</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C104" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D104" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F104" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G104" s="2" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" t="s">
-        <v>294</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="D105" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="F105" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="G105" s="2" t="s">
-        <v>548</v>
+        <v>473</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>543</v>
       </c>
     </row>
   </sheetData>
@@ -6062,17 +4112,17 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>295</v>
+        <v>220</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>296</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>297</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -6082,7 +4132,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>298</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -6100,1232 +4150,1232 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>299</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>300</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>301</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>302</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>303</v>
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>304</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>305</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" t="s">
-        <v>306</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>307</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>308</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>309</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>310</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:1">
       <c r="A13" t="s">
-        <v>311</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>312</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:1">
       <c r="A15" t="s">
-        <v>313</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:1">
       <c r="A16" t="s">
-        <v>314</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" t="s">
-        <v>315</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" t="s">
-        <v>316</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" t="s">
-        <v>317</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" t="s">
-        <v>318</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>319</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" t="s">
-        <v>320</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" t="s">
-        <v>321</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>322</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>323</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>324</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" t="s">
-        <v>325</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" t="s">
-        <v>326</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" t="s">
-        <v>327</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" t="s">
-        <v>328</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" t="s">
-        <v>329</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>330</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>331</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>332</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>333</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>334</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>335</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>336</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>337</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>338</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>339</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>340</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>341</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>342</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>343</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>344</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>345</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>346</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>347</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>348</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>349</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>350</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>351</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>352</v>
+        <v>277</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>353</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>354</v>
+        <v>279</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>355</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>356</v>
+        <v>281</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>357</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>358</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>359</v>
+        <v>284</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>360</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>361</v>
+        <v>286</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>362</v>
+        <v>287</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>363</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>364</v>
+        <v>289</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>365</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>366</v>
+        <v>291</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>367</v>
+        <v>292</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>368</v>
+        <v>293</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>369</v>
+        <v>294</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>370</v>
+        <v>295</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>371</v>
+        <v>296</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>372</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>373</v>
+        <v>298</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>374</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>375</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>376</v>
+        <v>301</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>377</v>
+        <v>302</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>378</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" spans="1:1">
       <c r="A81" t="s">
-        <v>379</v>
+        <v>304</v>
       </c>
     </row>
     <row r="82" spans="1:1">
       <c r="A82" t="s">
-        <v>380</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83" spans="1:1">
       <c r="A83" t="s">
-        <v>381</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84" spans="1:1">
       <c r="A84" t="s">
-        <v>382</v>
+        <v>307</v>
       </c>
     </row>
     <row r="85" spans="1:1">
       <c r="A85" t="s">
-        <v>383</v>
+        <v>308</v>
       </c>
     </row>
     <row r="86" spans="1:1">
       <c r="A86" t="s">
-        <v>384</v>
+        <v>309</v>
       </c>
     </row>
     <row r="87" spans="1:1">
       <c r="A87" t="s">
-        <v>385</v>
+        <v>310</v>
       </c>
     </row>
     <row r="88" spans="1:1">
       <c r="A88" t="s">
-        <v>386</v>
+        <v>311</v>
       </c>
     </row>
     <row r="89" spans="1:1">
       <c r="A89" t="s">
-        <v>387</v>
+        <v>312</v>
       </c>
     </row>
     <row r="90" spans="1:1">
       <c r="A90" t="s">
-        <v>388</v>
+        <v>313</v>
       </c>
     </row>
     <row r="91" spans="1:1">
       <c r="A91" t="s">
-        <v>389</v>
+        <v>314</v>
       </c>
     </row>
     <row r="92" spans="1:1">
       <c r="A92" t="s">
-        <v>390</v>
+        <v>315</v>
       </c>
     </row>
     <row r="93" spans="1:1">
       <c r="A93" t="s">
-        <v>391</v>
+        <v>316</v>
       </c>
     </row>
     <row r="94" spans="1:1">
       <c r="A94" t="s">
-        <v>392</v>
+        <v>317</v>
       </c>
     </row>
     <row r="95" spans="1:1">
       <c r="A95" t="s">
-        <v>393</v>
+        <v>318</v>
       </c>
     </row>
     <row r="96" spans="1:1">
       <c r="A96" t="s">
-        <v>394</v>
+        <v>319</v>
       </c>
     </row>
     <row r="97" spans="1:1">
       <c r="A97" t="s">
-        <v>395</v>
+        <v>320</v>
       </c>
     </row>
     <row r="98" spans="1:1">
       <c r="A98" t="s">
-        <v>396</v>
+        <v>321</v>
       </c>
     </row>
     <row r="99" spans="1:1">
       <c r="A99" t="s">
-        <v>397</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" spans="1:1">
       <c r="A100" t="s">
-        <v>398</v>
+        <v>323</v>
       </c>
     </row>
     <row r="101" spans="1:1">
       <c r="A101" t="s">
-        <v>399</v>
+        <v>324</v>
       </c>
     </row>
     <row r="102" spans="1:1">
       <c r="A102" t="s">
-        <v>400</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" spans="1:1">
       <c r="A103" t="s">
-        <v>401</v>
+        <v>326</v>
       </c>
     </row>
     <row r="104" spans="1:1">
       <c r="A104" t="s">
-        <v>402</v>
+        <v>327</v>
       </c>
     </row>
     <row r="105" spans="1:1">
       <c r="A105" t="s">
-        <v>403</v>
+        <v>328</v>
       </c>
     </row>
     <row r="106" spans="1:1">
       <c r="A106" t="s">
-        <v>404</v>
+        <v>329</v>
       </c>
     </row>
     <row r="107" spans="1:1">
       <c r="A107" t="s">
-        <v>405</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" spans="1:1">
       <c r="A108" t="s">
-        <v>406</v>
+        <v>331</v>
       </c>
     </row>
     <row r="109" spans="1:1">
       <c r="A109" t="s">
-        <v>407</v>
+        <v>332</v>
       </c>
     </row>
     <row r="110" spans="1:1">
       <c r="A110" t="s">
-        <v>408</v>
+        <v>333</v>
       </c>
     </row>
     <row r="111" spans="1:1">
       <c r="A111" t="s">
-        <v>409</v>
+        <v>334</v>
       </c>
     </row>
     <row r="112" spans="1:1">
       <c r="A112" t="s">
-        <v>410</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113" spans="1:1">
       <c r="A113" t="s">
-        <v>411</v>
+        <v>336</v>
       </c>
     </row>
     <row r="114" spans="1:1">
       <c r="A114" t="s">
-        <v>412</v>
+        <v>337</v>
       </c>
     </row>
     <row r="115" spans="1:1">
       <c r="A115" t="s">
-        <v>413</v>
+        <v>338</v>
       </c>
     </row>
     <row r="116" spans="1:1">
       <c r="A116" t="s">
-        <v>414</v>
+        <v>339</v>
       </c>
     </row>
     <row r="117" spans="1:1">
       <c r="A117" t="s">
-        <v>415</v>
+        <v>340</v>
       </c>
     </row>
     <row r="118" spans="1:1">
       <c r="A118" t="s">
-        <v>416</v>
+        <v>341</v>
       </c>
     </row>
     <row r="119" spans="1:1">
       <c r="A119" t="s">
-        <v>417</v>
+        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:1">
       <c r="A120" t="s">
-        <v>418</v>
+        <v>343</v>
       </c>
     </row>
     <row r="121" spans="1:1">
       <c r="A121" t="s">
-        <v>419</v>
+        <v>344</v>
       </c>
     </row>
     <row r="122" spans="1:1">
       <c r="A122" t="s">
-        <v>420</v>
+        <v>345</v>
       </c>
     </row>
     <row r="123" spans="1:1">
       <c r="A123" t="s">
-        <v>421</v>
+        <v>346</v>
       </c>
     </row>
     <row r="124" spans="1:1">
       <c r="A124" t="s">
-        <v>422</v>
+        <v>347</v>
       </c>
     </row>
     <row r="125" spans="1:1">
       <c r="A125" t="s">
-        <v>423</v>
+        <v>348</v>
       </c>
     </row>
     <row r="126" spans="1:1">
       <c r="A126" t="s">
-        <v>424</v>
+        <v>349</v>
       </c>
     </row>
     <row r="127" spans="1:1">
       <c r="A127" t="s">
-        <v>425</v>
+        <v>350</v>
       </c>
     </row>
     <row r="128" spans="1:1">
       <c r="A128" t="s">
-        <v>426</v>
+        <v>351</v>
       </c>
     </row>
     <row r="129" spans="1:1">
       <c r="A129" t="s">
-        <v>427</v>
+        <v>352</v>
       </c>
     </row>
     <row r="130" spans="1:1">
       <c r="A130" t="s">
-        <v>428</v>
+        <v>353</v>
       </c>
     </row>
     <row r="131" spans="1:1">
       <c r="A131" t="s">
-        <v>429</v>
+        <v>354</v>
       </c>
     </row>
     <row r="132" spans="1:1">
       <c r="A132" t="s">
-        <v>430</v>
+        <v>355</v>
       </c>
     </row>
     <row r="133" spans="1:1">
       <c r="A133" t="s">
-        <v>431</v>
+        <v>356</v>
       </c>
     </row>
     <row r="134" spans="1:1">
       <c r="A134" t="s">
-        <v>432</v>
+        <v>357</v>
       </c>
     </row>
     <row r="135" spans="1:1">
       <c r="A135" t="s">
-        <v>433</v>
+        <v>358</v>
       </c>
     </row>
     <row r="136" spans="1:1">
       <c r="A136" t="s">
-        <v>434</v>
+        <v>359</v>
       </c>
     </row>
     <row r="137" spans="1:1">
       <c r="A137" t="s">
-        <v>435</v>
+        <v>360</v>
       </c>
     </row>
     <row r="138" spans="1:1">
       <c r="A138" t="s">
-        <v>436</v>
+        <v>361</v>
       </c>
     </row>
     <row r="139" spans="1:1">
       <c r="A139" t="s">
-        <v>437</v>
+        <v>362</v>
       </c>
     </row>
     <row r="140" spans="1:1">
       <c r="A140" t="s">
-        <v>438</v>
+        <v>363</v>
       </c>
     </row>
     <row r="141" spans="1:1">
       <c r="A141" t="s">
-        <v>439</v>
+        <v>364</v>
       </c>
     </row>
     <row r="142" spans="1:1">
       <c r="A142" t="s">
-        <v>440</v>
+        <v>365</v>
       </c>
     </row>
     <row r="143" spans="1:1">
       <c r="A143" t="s">
-        <v>441</v>
+        <v>366</v>
       </c>
     </row>
     <row r="144" spans="1:1">
       <c r="A144" t="s">
-        <v>442</v>
+        <v>367</v>
       </c>
     </row>
     <row r="145" spans="1:1">
       <c r="A145" t="s">
-        <v>443</v>
+        <v>368</v>
       </c>
     </row>
     <row r="146" spans="1:1">
       <c r="A146" t="s">
-        <v>444</v>
+        <v>369</v>
       </c>
     </row>
     <row r="147" spans="1:1">
       <c r="A147" t="s">
-        <v>445</v>
+        <v>370</v>
       </c>
     </row>
     <row r="148" spans="1:1">
       <c r="A148" t="s">
-        <v>446</v>
+        <v>371</v>
       </c>
     </row>
     <row r="149" spans="1:1">
       <c r="A149" t="s">
-        <v>447</v>
+        <v>372</v>
       </c>
     </row>
     <row r="150" spans="1:1">
       <c r="A150" t="s">
-        <v>448</v>
+        <v>373</v>
       </c>
     </row>
     <row r="151" spans="1:1">
       <c r="A151" t="s">
-        <v>449</v>
+        <v>374</v>
       </c>
     </row>
     <row r="152" spans="1:1">
       <c r="A152" t="s">
-        <v>450</v>
+        <v>375</v>
       </c>
     </row>
     <row r="153" spans="1:1">
       <c r="A153" t="s">
-        <v>451</v>
+        <v>376</v>
       </c>
     </row>
     <row r="154" spans="1:1">
       <c r="A154" t="s">
-        <v>452</v>
+        <v>377</v>
       </c>
     </row>
     <row r="155" spans="1:1">
       <c r="A155" t="s">
-        <v>453</v>
+        <v>378</v>
       </c>
     </row>
     <row r="156" spans="1:1">
       <c r="A156" t="s">
-        <v>454</v>
+        <v>379</v>
       </c>
     </row>
     <row r="157" spans="1:1">
       <c r="A157" t="s">
-        <v>455</v>
+        <v>380</v>
       </c>
     </row>
     <row r="158" spans="1:1">
       <c r="A158" t="s">
-        <v>456</v>
+        <v>381</v>
       </c>
     </row>
     <row r="159" spans="1:1">
       <c r="A159" t="s">
-        <v>457</v>
+        <v>382</v>
       </c>
     </row>
     <row r="160" spans="1:1">
       <c r="A160" t="s">
-        <v>458</v>
+        <v>383</v>
       </c>
     </row>
     <row r="161" spans="1:1">
       <c r="A161" t="s">
-        <v>459</v>
+        <v>384</v>
       </c>
     </row>
     <row r="162" spans="1:1">
       <c r="A162" t="s">
-        <v>460</v>
+        <v>385</v>
       </c>
     </row>
     <row r="163" spans="1:1">
       <c r="A163" t="s">
-        <v>461</v>
+        <v>386</v>
       </c>
     </row>
     <row r="164" spans="1:1">
       <c r="A164" t="s">
-        <v>462</v>
+        <v>387</v>
       </c>
     </row>
     <row r="165" spans="1:1">
       <c r="A165" t="s">
-        <v>463</v>
+        <v>388</v>
       </c>
     </row>
     <row r="166" spans="1:1">
       <c r="A166" t="s">
-        <v>464</v>
+        <v>389</v>
       </c>
     </row>
     <row r="167" spans="1:1">
       <c r="A167" t="s">
-        <v>465</v>
+        <v>390</v>
       </c>
     </row>
     <row r="168" spans="1:1">
       <c r="A168" t="s">
-        <v>466</v>
+        <v>391</v>
       </c>
     </row>
     <row r="169" spans="1:1">
       <c r="A169" t="s">
-        <v>467</v>
+        <v>392</v>
       </c>
     </row>
     <row r="170" spans="1:1">
       <c r="A170" t="s">
-        <v>468</v>
+        <v>393</v>
       </c>
     </row>
     <row r="171" spans="1:1">
       <c r="A171" t="s">
-        <v>469</v>
+        <v>394</v>
       </c>
     </row>
     <row r="172" spans="1:1">
       <c r="A172" t="s">
-        <v>470</v>
+        <v>395</v>
       </c>
     </row>
     <row r="173" spans="1:1">
       <c r="A173" t="s">
-        <v>471</v>
+        <v>396</v>
       </c>
     </row>
     <row r="174" spans="1:1">
       <c r="A174" t="s">
-        <v>472</v>
+        <v>397</v>
       </c>
     </row>
     <row r="175" spans="1:1">
       <c r="A175" t="s">
-        <v>473</v>
+        <v>398</v>
       </c>
     </row>
     <row r="176" spans="1:1">
       <c r="A176" t="s">
-        <v>474</v>
+        <v>399</v>
       </c>
     </row>
     <row r="177" spans="1:1">
       <c r="A177" t="s">
-        <v>475</v>
+        <v>400</v>
       </c>
     </row>
     <row r="178" spans="1:1">
       <c r="A178" t="s">
-        <v>476</v>
+        <v>401</v>
       </c>
     </row>
     <row r="179" spans="1:1">
       <c r="A179" t="s">
-        <v>477</v>
+        <v>402</v>
       </c>
     </row>
     <row r="180" spans="1:1">
       <c r="A180" t="s">
-        <v>478</v>
+        <v>403</v>
       </c>
     </row>
     <row r="181" spans="1:1">
       <c r="A181" t="s">
-        <v>479</v>
+        <v>404</v>
       </c>
     </row>
     <row r="182" spans="1:1">
       <c r="A182" t="s">
-        <v>480</v>
+        <v>405</v>
       </c>
     </row>
     <row r="183" spans="1:1">
       <c r="A183" t="s">
-        <v>481</v>
+        <v>406</v>
       </c>
     </row>
     <row r="184" spans="1:1">
       <c r="A184" t="s">
-        <v>482</v>
+        <v>407</v>
       </c>
     </row>
     <row r="185" spans="1:1">
       <c r="A185" t="s">
-        <v>483</v>
+        <v>408</v>
       </c>
     </row>
     <row r="186" spans="1:1">
       <c r="A186" t="s">
-        <v>484</v>
+        <v>409</v>
       </c>
     </row>
     <row r="187" spans="1:1">
       <c r="A187" t="s">
-        <v>485</v>
+        <v>410</v>
       </c>
     </row>
     <row r="188" spans="1:1">
       <c r="A188" t="s">
-        <v>486</v>
+        <v>411</v>
       </c>
     </row>
     <row r="189" spans="1:1">
       <c r="A189" t="s">
-        <v>487</v>
+        <v>412</v>
       </c>
     </row>
     <row r="190" spans="1:1">
       <c r="A190" t="s">
-        <v>488</v>
+        <v>413</v>
       </c>
     </row>
     <row r="191" spans="1:1">
       <c r="A191" t="s">
-        <v>489</v>
+        <v>414</v>
       </c>
     </row>
     <row r="192" spans="1:1">
       <c r="A192" t="s">
-        <v>490</v>
+        <v>415</v>
       </c>
     </row>
     <row r="193" spans="1:1">
       <c r="A193" t="s">
-        <v>491</v>
+        <v>416</v>
       </c>
     </row>
     <row r="194" spans="1:1">
       <c r="A194" t="s">
-        <v>492</v>
+        <v>417</v>
       </c>
     </row>
     <row r="195" spans="1:1">
       <c r="A195" t="s">
-        <v>493</v>
+        <v>418</v>
       </c>
     </row>
     <row r="196" spans="1:1">
       <c r="A196" t="s">
-        <v>494</v>
+        <v>419</v>
       </c>
     </row>
     <row r="197" spans="1:1">
       <c r="A197" t="s">
-        <v>495</v>
+        <v>420</v>
       </c>
     </row>
     <row r="198" spans="1:1">
       <c r="A198" t="s">
-        <v>496</v>
+        <v>421</v>
       </c>
     </row>
     <row r="199" spans="1:1">
       <c r="A199" t="s">
-        <v>497</v>
+        <v>422</v>
       </c>
     </row>
     <row r="200" spans="1:1">
       <c r="A200" t="s">
-        <v>498</v>
+        <v>423</v>
       </c>
     </row>
     <row r="201" spans="1:1">
       <c r="A201" t="s">
-        <v>499</v>
+        <v>424</v>
       </c>
     </row>
     <row r="202" spans="1:1">
       <c r="A202" t="s">
-        <v>500</v>
+        <v>425</v>
       </c>
     </row>
     <row r="203" spans="1:1">
       <c r="A203" t="s">
-        <v>501</v>
+        <v>426</v>
       </c>
     </row>
     <row r="204" spans="1:1">
       <c r="A204" t="s">
-        <v>502</v>
+        <v>427</v>
       </c>
     </row>
     <row r="205" spans="1:1">
       <c r="A205" t="s">
-        <v>503</v>
+        <v>428</v>
       </c>
     </row>
     <row r="206" spans="1:1">
       <c r="A206" t="s">
-        <v>504</v>
+        <v>429</v>
       </c>
     </row>
     <row r="207" spans="1:1">
       <c r="A207" t="s">
-        <v>505</v>
+        <v>430</v>
       </c>
     </row>
     <row r="208" spans="1:1">
       <c r="A208" t="s">
-        <v>506</v>
+        <v>431</v>
       </c>
     </row>
     <row r="209" spans="1:1">
       <c r="A209" t="s">
-        <v>507</v>
+        <v>432</v>
       </c>
     </row>
     <row r="210" spans="1:1">
       <c r="A210" t="s">
-        <v>508</v>
+        <v>433</v>
       </c>
     </row>
     <row r="211" spans="1:1">
       <c r="A211" t="s">
-        <v>509</v>
+        <v>434</v>
       </c>
     </row>
     <row r="212" spans="1:1">
       <c r="A212" t="s">
-        <v>510</v>
+        <v>435</v>
       </c>
     </row>
     <row r="213" spans="1:1">
       <c r="A213" t="s">
-        <v>511</v>
+        <v>436</v>
       </c>
     </row>
     <row r="214" spans="1:1">
       <c r="A214" t="s">
-        <v>512</v>
+        <v>437</v>
       </c>
     </row>
     <row r="215" spans="1:1">
       <c r="A215" t="s">
-        <v>513</v>
+        <v>438</v>
       </c>
     </row>
     <row r="216" spans="1:1">
       <c r="A216" t="s">
-        <v>514</v>
+        <v>439</v>
       </c>
     </row>
     <row r="217" spans="1:1">
       <c r="A217" t="s">
-        <v>515</v>
+        <v>440</v>
       </c>
     </row>
     <row r="218" spans="1:1">
       <c r="A218" t="s">
-        <v>516</v>
+        <v>441</v>
       </c>
     </row>
     <row r="219" spans="1:1">
       <c r="A219" t="s">
-        <v>517</v>
+        <v>442</v>
       </c>
     </row>
     <row r="220" spans="1:1">
       <c r="A220" t="s">
-        <v>518</v>
+        <v>443</v>
       </c>
     </row>
     <row r="221" spans="1:1">
       <c r="A221" t="s">
-        <v>519</v>
+        <v>444</v>
       </c>
     </row>
     <row r="222" spans="1:1">
       <c r="A222" t="s">
-        <v>520</v>
+        <v>445</v>
       </c>
     </row>
     <row r="223" spans="1:1">
       <c r="A223" t="s">
-        <v>521</v>
+        <v>446</v>
       </c>
     </row>
     <row r="224" spans="1:1">
       <c r="A224" t="s">
-        <v>522</v>
+        <v>447</v>
       </c>
     </row>
     <row r="225" spans="1:1">
       <c r="A225" t="s">
-        <v>523</v>
+        <v>448</v>
       </c>
     </row>
     <row r="226" spans="1:1">
       <c r="A226" t="s">
-        <v>524</v>
+        <v>449</v>
       </c>
     </row>
     <row r="227" spans="1:1">
       <c r="A227" t="s">
-        <v>525</v>
+        <v>450</v>
       </c>
     </row>
     <row r="228" spans="1:1">
       <c r="A228" t="s">
-        <v>526</v>
+        <v>451</v>
       </c>
     </row>
     <row r="229" spans="1:1">
       <c r="A229" t="s">
-        <v>527</v>
+        <v>452</v>
       </c>
     </row>
     <row r="230" spans="1:1">
       <c r="A230" t="s">
-        <v>528</v>
+        <v>453</v>
       </c>
     </row>
     <row r="231" spans="1:1">
       <c r="A231" t="s">
-        <v>529</v>
+        <v>454</v>
       </c>
     </row>
     <row r="232" spans="1:1">
       <c r="A232" t="s">
-        <v>530</v>
+        <v>455</v>
       </c>
     </row>
     <row r="233" spans="1:1">
       <c r="A233" t="s">
-        <v>531</v>
+        <v>456</v>
       </c>
     </row>
     <row r="234" spans="1:1">
       <c r="A234" t="s">
-        <v>532</v>
+        <v>457</v>
       </c>
     </row>
     <row r="235" spans="1:1">
       <c r="A235" t="s">
-        <v>533</v>
+        <v>458</v>
       </c>
     </row>
     <row r="236" spans="1:1">
       <c r="A236" t="s">
-        <v>534</v>
+        <v>459</v>
       </c>
     </row>
     <row r="237" spans="1:1">
       <c r="A237" t="s">
-        <v>535</v>
+        <v>460</v>
       </c>
     </row>
     <row r="238" spans="1:1">
       <c r="A238" t="s">
-        <v>536</v>
+        <v>461</v>
       </c>
     </row>
     <row r="239" spans="1:1">
       <c r="A239" t="s">
-        <v>537</v>
+        <v>462</v>
       </c>
     </row>
     <row r="240" spans="1:1">
       <c r="A240" t="s">
-        <v>538</v>
+        <v>463</v>
       </c>
     </row>
     <row r="241" spans="1:1">
       <c r="A241" t="s">
-        <v>539</v>
+        <v>464</v>
       </c>
     </row>
     <row r="242" spans="1:1">
       <c r="A242" t="s">
-        <v>540</v>
+        <v>465</v>
       </c>
     </row>
     <row r="243" spans="1:1">
       <c r="A243" t="s">
-        <v>541</v>
+        <v>466</v>
       </c>
     </row>
     <row r="244" spans="1:1">
       <c r="A244" t="s">
-        <v>542</v>
+        <v>467</v>
       </c>
     </row>
     <row r="245" spans="1:1">
       <c r="A245" t="s">
-        <v>543</v>
+        <v>468</v>
       </c>
     </row>
     <row r="246" spans="1:1">
       <c r="A246" t="s">
-        <v>544</v>
+        <v>469</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Expanded store potential items tests
</commit_message>
<xml_diff>
--- a/vfBattleTechMod-ProcGenStores-Test/res/xlrp-store-content.xlsx
+++ b/vfBattleTechMod-ProcGenStores-Test/res/xlrp-store-content.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen Weistra\gitrepos\vfBattleTechMod-Core\vfBattleTechMod-ProcGenStores-Test\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F8EBE0-0965-44E4-94DF-7FB8803BEA69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF98712-98B4-4654-9B87-B23B5F5BD50A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4275" yWindow="-21720" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3386,7 +3386,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3770,8 +3770,11 @@
       <c r="G16" s="2" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="H16" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>206</v>
       </c>
@@ -3794,7 +3797,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>207</v>
       </c>
@@ -3817,7 +3820,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>208</v>
       </c>
@@ -3840,7 +3843,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>209</v>
       </c>
@@ -3863,7 +3866,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>210</v>
       </c>
@@ -3886,7 +3889,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>211</v>
       </c>
@@ -3909,7 +3912,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>212</v>
       </c>
@@ -3932,7 +3935,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>213</v>
       </c>
@@ -3955,7 +3958,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>214</v>
       </c>
@@ -3978,7 +3981,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>215</v>
       </c>
@@ -4001,7 +4004,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>216</v>
       </c>
@@ -4024,7 +4027,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>217</v>
       </c>
@@ -4047,7 +4050,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>218</v>
       </c>
@@ -4070,7 +4073,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>219</v>
       </c>
@@ -4091,9 +4094,6 @@
       </c>
       <c r="G30" s="2" t="s">
         <v>473</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>543</v>
       </c>
     </row>
   </sheetData>

</xml_diff>